<commit_message>
Changes to be committed: 	modified:   Sprints.ods 	modified:   Sprints.xlsx
</commit_message>
<xml_diff>
--- a/Sprints.xlsx
+++ b/Sprints.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t xml:space="preserve">Backlog</t>
   </si>
@@ -28,12 +28,12 @@
     <t xml:space="preserve">Historia</t>
   </si>
   <si>
-    <t xml:space="preserve">Sprint</t>
-  </si>
-  <si>
     <t xml:space="preserve">Tema</t>
   </si>
   <si>
+    <t xml:space="preserve">Tiempo (planning poker)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Renderizar páginas web en cuadros de visualización dentro de una misma</t>
   </si>
   <si>
@@ -43,7 +43,7 @@
     <t xml:space="preserve">-Funcionalidad basica</t>
   </si>
   <si>
-    <t xml:space="preserve">-Hacer backend y base de datos(BBDD), con la función de añadir publicación de paginas y  categorizarlas con nombre/ID/fecha/creador/likes/comentarios</t>
+    <t xml:space="preserve">-Hacer backend y base de datos(BBDD), con la función de añadir publicación de paginas y  categorizarlas con nombre/ID/fecha/creador/likes/comentarios </t>
   </si>
   <si>
     <t xml:space="preserve">“Como desarrollador yo quiero un sistema para guardar publicaciones en una base de datos para poder luego ser usada por un cliente en una interfaz en una página en el frontend”                                                                        “Como desarrollador yo quiero que cada  publicación tenga información extra para fácilmente añadir nuevas características mas adelante”</t>
@@ -143,6 +143,9 @@
   </si>
   <si>
     <t xml:space="preserve">“Como usuario yo quiero que se puedan ver los likes y comentarios de una publicación para saber si se habla/hablo de la publicación (con la cantidad de comentarios) y si fue por polémica o por que fue bien hecha (por la cantidad de likes)”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">½</t>
   </si>
   <si>
     <t xml:space="preserve">-Añadir funcionalidad a pagina principal de mostrar publicaciones con mas likes</t>
@@ -155,14 +158,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -184,16 +189,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
-      <sz val="96"/>
+      <sz val="20"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="80"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -234,7 +236,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -242,6 +244,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -268,7 +298,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -277,80 +307,108 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -426,23 +484,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="71.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="50.99"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="41.13"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="41.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -452,14 +508,15 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="1"/>
+      <c r="D1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="E1" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -467,204 +524,240 @@
         <v>5</v>
       </c>
       <c r="C2" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>6</v>
       </c>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="70.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-    </row>
-    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
+      <c r="C3" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="6"/>
+    </row>
+    <row r="4" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C4" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="6"/>
+    </row>
+    <row r="5" customFormat="false" ht="81.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-    </row>
-    <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="s">
+      <c r="C5" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="6"/>
+    </row>
+    <row r="6" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="9" t="n">
+      <c r="C6" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="6"/>
+    </row>
+    <row r="7" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="D7" s="12"/>
+      <c r="E7" s="6"/>
+    </row>
+    <row r="8" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="D8" s="12"/>
+      <c r="E8" s="6"/>
+    </row>
+    <row r="9" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="D9" s="12"/>
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="15" t="n">
+        <v>3</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="6"/>
+    </row>
+    <row r="11" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="15" t="n">
+        <v>13</v>
+      </c>
+      <c r="D11" s="16"/>
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="16"/>
+      <c r="E12" s="6"/>
+    </row>
+    <row r="13" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="20" t="n">
+        <v>40</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="20" t="n">
+        <v>13</v>
+      </c>
+      <c r="D14" s="21"/>
+      <c r="E14" s="6"/>
+    </row>
+    <row r="15" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="25" t="n">
+        <v>5</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="6"/>
+    </row>
+    <row r="16" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="25" t="n">
         <v>2</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-    </row>
-    <row r="8" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-    </row>
-    <row r="9" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-    </row>
-    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="12" t="n">
+      <c r="D16" s="26"/>
+      <c r="E16" s="6"/>
+    </row>
+    <row r="17" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="26"/>
+      <c r="E17" s="6"/>
+    </row>
+    <row r="18" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="25" t="n">
         <v>3</v>
       </c>
-      <c r="D10" s="13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-    </row>
-    <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-    </row>
-    <row r="13" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="16" t="n">
-        <v>4</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-    </row>
-    <row r="15" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="20" t="n">
-        <v>5</v>
-      </c>
-      <c r="D15" s="18" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-    </row>
-    <row r="17" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-    </row>
-    <row r="18" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="C2:C5"/>
+  <mergeCells count="5">
     <mergeCell ref="D2:D5"/>
-    <mergeCell ref="C6:C9"/>
     <mergeCell ref="D6:D9"/>
-    <mergeCell ref="C10:C12"/>
     <mergeCell ref="D10:D12"/>
-    <mergeCell ref="C13:C14"/>
     <mergeCell ref="D13:D14"/>
-    <mergeCell ref="C15:C18"/>
     <mergeCell ref="D15:D18"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>

</xml_diff>